<commit_message>
updated BOM and RS component
</commit_message>
<xml_diff>
--- a/Hardware/StmPulse-V1-G498043-bom.xlsx
+++ b/Hardware/StmPulse-V1-G498043-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyc/Documents/Arduino/STM/STMPulseOLED/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7E85F729-0D94-B845-BC92-AA0DE5AC422C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A7A1446B-DFF5-D140-AB01-A42051816614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="4620" yWindow="460" windowWidth="28040" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="StmPulse-V1-G498043-bom" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
   <si>
     <t>Library</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Diode</t>
   </si>
   <si>
-    <t>1N4001</t>
-  </si>
-  <si>
     <t>SMADIODE</t>
   </si>
   <si>
@@ -344,13 +341,58 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n 14</t>
+  </si>
+  <si>
+    <t>Y 8</t>
+  </si>
+  <si>
+    <t>Y 2</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">223-0562 / 125-1189 </t>
+  </si>
+  <si>
+    <t>y 1</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Stth102a</t>
+  </si>
+  <si>
+    <t>Y 10</t>
+  </si>
+  <si>
+    <t>812-3508</t>
+  </si>
+  <si>
+    <t>737-9704</t>
+  </si>
+  <si>
+    <t>223-0821</t>
+  </si>
+  <si>
+    <t>828-1783</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -484,6 +526,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -827,8 +875,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1187,7 +1236,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -1256,93 +1305,111 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1350,412 +1417,481 @@
         <v>16</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>86</v>
+      </c>
+      <c r="J10" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>56</v>
       </c>
-      <c r="F12" t="s">
+      <c r="J12" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" t="s">
         <v>57</v>
       </c>
-      <c r="N12" t="s">
-        <v>58</v>
+      <c r="O12" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="D13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" t="s">
+      <c r="J13" t="s">
+        <v>106</v>
+      </c>
+      <c r="N13" t="s">
         <v>61</v>
-      </c>
-      <c r="N13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>90</v>
+      </c>
+      <c r="J14" t="s">
+        <v>108</v>
+      </c>
+      <c r="O14" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" t="s">
-        <v>67</v>
+        <v>90</v>
+      </c>
+      <c r="J15" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="J16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>90</v>
+      </c>
+      <c r="J17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18">
-        <v>1755108</v>
-      </c>
-      <c r="L18" t="s">
-        <v>80</v>
-      </c>
-      <c r="M18" t="s">
-        <v>81</v>
-      </c>
-      <c r="O18" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>83</v>
+        <v>90</v>
+      </c>
+      <c r="J18" t="s">
+        <v>115</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>77</v>
+      </c>
+      <c r="I19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19">
+        <v>1755108</v>
+      </c>
+      <c r="L19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" t="s">
+        <v>80</v>
+      </c>
+      <c r="O19" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="J20" t="s">
+        <v>110</v>
+      </c>
+      <c r="P20" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" t="s">
+        <v>107</v>
+      </c>
+      <c r="O21" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>107</v>
+      </c>
+      <c r="O22" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>91</v>
+        <v>29</v>
+      </c>
+      <c r="J24" t="s">
+        <v>106</v>
+      </c>
+      <c r="O24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
-      </c>
-      <c r="P25" t="s">
-        <v>105</v>
+        <v>29</v>
+      </c>
+      <c r="J25" t="s">
+        <v>111</v>
+      </c>
+      <c r="O25" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q25">
+    <sortCondition ref="C2:C25"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>